<commit_message>
used: finish LP bot used to finish lost KW99
</commit_message>
<xml_diff>
--- a/Open-LPs - pé.xlsx
+++ b/Open-LPs - pé.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F79E12A-AE75-43A8-9DBD-F0ACD32BFEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D188510C-AB41-4180-AF8E-D6853F74783C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,117 +20,180 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>LP</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>LP-045068</t>
-  </si>
-  <si>
-    <t>LP-045256</t>
-  </si>
-  <si>
-    <t>LP-046955</t>
-  </si>
-  <si>
-    <t>LP-047335</t>
-  </si>
-  <si>
-    <t>LP-047467</t>
-  </si>
-  <si>
-    <t>LP-047773</t>
-  </si>
-  <si>
-    <t>LP-047836</t>
-  </si>
-  <si>
-    <t>LP-047837</t>
-  </si>
-  <si>
-    <t>LP-047843</t>
-  </si>
-  <si>
-    <t>LP-047889</t>
-  </si>
-  <si>
-    <t>LP-048138</t>
-  </si>
-  <si>
-    <t>LP-048139</t>
-  </si>
-  <si>
-    <t>LP-048156</t>
-  </si>
-  <si>
-    <t>LP-048187</t>
-  </si>
-  <si>
-    <t>LP-048188</t>
-  </si>
-  <si>
-    <t>LP-048221</t>
-  </si>
-  <si>
-    <t>LP-048279</t>
-  </si>
-  <si>
-    <t>LP-048379</t>
-  </si>
-  <si>
-    <t>LP-048390</t>
-  </si>
-  <si>
-    <t>LP-048643</t>
-  </si>
-  <si>
-    <t>LP-048732</t>
-  </si>
-  <si>
-    <t>LP-048733</t>
-  </si>
-  <si>
-    <t>LP-048999</t>
-  </si>
-  <si>
-    <t>LP-049034</t>
-  </si>
-  <si>
-    <t>LP-049039</t>
-  </si>
-  <si>
-    <t>LP-049120</t>
-  </si>
-  <si>
-    <t>LP-049141</t>
-  </si>
-  <si>
-    <t>LP-049216</t>
-  </si>
-  <si>
-    <t>LP-049627</t>
-  </si>
-  <si>
-    <t>LP-049650</t>
-  </si>
-  <si>
-    <t>LP-049673</t>
-  </si>
-  <si>
-    <t>LP-049801</t>
-  </si>
-  <si>
-    <t>LP-049831</t>
-  </si>
-  <si>
-    <t>LP-048644</t>
-  </si>
-  <si>
-    <t>LP-049326</t>
+    <t>LP-042432</t>
+  </si>
+  <si>
+    <t>LP-043478</t>
+  </si>
+  <si>
+    <t>LP-045475</t>
+  </si>
+  <si>
+    <t>LP-046179</t>
+  </si>
+  <si>
+    <t>LP-046670</t>
+  </si>
+  <si>
+    <t>LP-047185</t>
+  </si>
+  <si>
+    <t>LP-047204</t>
+  </si>
+  <si>
+    <t>LP-047489</t>
+  </si>
+  <si>
+    <t>LP-047515</t>
+  </si>
+  <si>
+    <t>LP-047522</t>
+  </si>
+  <si>
+    <t>LP-048148</t>
+  </si>
+  <si>
+    <t>LP-048174</t>
+  </si>
+  <si>
+    <t>LP-048190</t>
+  </si>
+  <si>
+    <t>LP-048192</t>
+  </si>
+  <si>
+    <t>LP-048349</t>
+  </si>
+  <si>
+    <t>LP-048365</t>
+  </si>
+  <si>
+    <t>LP-048371</t>
+  </si>
+  <si>
+    <t>LP-048387</t>
+  </si>
+  <si>
+    <t>LP-048391</t>
+  </si>
+  <si>
+    <t>LP-048424</t>
+  </si>
+  <si>
+    <t>LP-048425</t>
+  </si>
+  <si>
+    <t>LP-048651</t>
+  </si>
+  <si>
+    <t>LP-048652</t>
+  </si>
+  <si>
+    <t>LP-048972</t>
+  </si>
+  <si>
+    <t>LP-048980</t>
+  </si>
+  <si>
+    <t>LP-048994</t>
+  </si>
+  <si>
+    <t>LP-049037</t>
+  </si>
+  <si>
+    <t>LP-049043</t>
+  </si>
+  <si>
+    <t>LP-049342</t>
+  </si>
+  <si>
+    <t>LP-049362</t>
+  </si>
+  <si>
+    <t>LP-049377</t>
+  </si>
+  <si>
+    <t>LP-049386</t>
+  </si>
+  <si>
+    <t>LP-049388</t>
+  </si>
+  <si>
+    <t>LP-049389</t>
+  </si>
+  <si>
+    <t>LP-049442</t>
+  </si>
+  <si>
+    <t>LP-049463</t>
+  </si>
+  <si>
+    <t>LP-049510</t>
+  </si>
+  <si>
+    <t>LP-049511</t>
+  </si>
+  <si>
+    <t>LP-049512</t>
+  </si>
+  <si>
+    <t>LP-049620</t>
+  </si>
+  <si>
+    <t>LP-049659</t>
+  </si>
+  <si>
+    <t>LP-049668</t>
+  </si>
+  <si>
+    <t>LP-049671</t>
+  </si>
+  <si>
+    <t>LP-049676</t>
+  </si>
+  <si>
+    <t>LP-049677</t>
+  </si>
+  <si>
+    <t>LP-049684</t>
+  </si>
+  <si>
+    <t>LP-049763</t>
+  </si>
+  <si>
+    <t>LP-049829</t>
+  </si>
+  <si>
+    <t>LP-049833</t>
+  </si>
+  <si>
+    <t>LP-049834</t>
+  </si>
+  <si>
+    <t>LP-049860</t>
+  </si>
+  <si>
+    <t>LP-050087</t>
+  </si>
+  <si>
+    <t>LP-048191</t>
+  </si>
+  <si>
+    <t>LP-048274</t>
+  </si>
+  <si>
+    <t>LP-048803</t>
+  </si>
+  <si>
+    <t>LP-049214</t>
+  </si>
+  <si>
+    <t>LP-049499</t>
   </si>
 </sst>
 </file>
@@ -493,197 +556,305 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:A58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A58"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>